<commit_message>
add monthly yearly functionality in customers and tax sections, add migration for add tax_duration col
</commit_message>
<xml_diff>
--- a/public/samples/company.xlsx
+++ b/public/samples/company.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name Khmer</t>
   </si>
@@ -62,13 +62,16 @@
   </si>
   <si>
     <t>Industry</t>
+  </si>
+  <si>
+    <t>Tax Duration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +598,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -673,6 +681,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -707,6 +716,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -882,16 +892,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -939,6 +949,9 @@
       </c>
       <c r="P1" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
export customers export Employees export Team Members adds ePhone text field in add customer adds children text field in employees adds children and e_phone columns migrations
</commit_message>
<xml_diff>
--- a/public/samples/company.xlsx
+++ b/public/samples/company.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name Khmer</t>
   </si>
@@ -65,13 +65,16 @@
   </si>
   <si>
     <t>Tax Duration</t>
+  </si>
+  <si>
+    <t>ePhone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,7 +684,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -716,7 +718,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -892,16 +893,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -945,12 +946,15 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>